<commit_message>
For the WK 3 to WK 4 Transitional, I am Staging, Pushing, and Committing my updated components, docs, and logs folders.
</commit_message>
<xml_diff>
--- a/logs/RitchieMichael_TimeEstimation.xlsx
+++ b/logs/RitchieMichael_TimeEstimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="460" windowWidth="22640" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="13060" yWindow="460" windowWidth="15740" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Michael Ritchie</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>The Burn-Up List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: The Week Ahead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Career Module: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: GoToTraining (GTT) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: Call to Action - Encouragement! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating with Clarity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating with Visual Tools </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: Research </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: Development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WK 3: Project &amp; Portfolio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Burn-Up List </t>
   </si>
 </sst>
 </file>
@@ -336,6 +366,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,15 +392,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,15 +670,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FN45"/>
+  <dimension ref="A1:FN54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.1640625" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="4" customWidth="1"/>
     <col min="3" max="5" width="16.1640625" style="16"/>
     <col min="6" max="170" width="16.1640625" style="6"/>
@@ -656,13 +686,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:170" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -830,13 +860,13 @@
       <c r="FN1" s="7"/>
     </row>
     <row r="2" spans="1:170" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1004,13 +1034,13 @@
       <c r="FN2" s="7"/>
     </row>
     <row r="3" spans="1:170" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1178,11 +1208,11 @@
       <c r="FN3" s="7"/>
     </row>
     <row r="4" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1779,11 +1809,11 @@
       </c>
     </row>
     <row r="22" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2200,11 +2230,11 @@
       </c>
     </row>
     <row r="39" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -2382,376 +2412,529 @@
     </row>
     <row r="41" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5"/>
-      <c r="AB42" s="5"/>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
-      <c r="AE42" s="5"/>
-      <c r="AF42" s="5"/>
-      <c r="AG42" s="5"/>
-      <c r="AH42" s="5"/>
-      <c r="AI42" s="5"/>
-      <c r="AJ42" s="5"/>
-      <c r="AK42" s="5"/>
-      <c r="AL42" s="5"/>
-      <c r="AM42" s="5"/>
-      <c r="AN42" s="5"/>
-      <c r="AO42" s="5"/>
-      <c r="AP42" s="5"/>
-      <c r="AQ42" s="5"/>
-      <c r="AR42" s="5"/>
-      <c r="AS42" s="5"/>
-      <c r="AT42" s="5"/>
-      <c r="AU42" s="5"/>
-      <c r="AV42" s="5"/>
-      <c r="AW42" s="5"/>
-      <c r="AX42" s="5"/>
-      <c r="AY42" s="5"/>
-      <c r="AZ42" s="5"/>
-      <c r="BA42" s="5"/>
-      <c r="BB42" s="5"/>
-      <c r="BC42" s="5"/>
-      <c r="BD42" s="5"/>
-      <c r="BE42" s="5"/>
-      <c r="BF42" s="5"/>
-      <c r="BG42" s="5"/>
-      <c r="BH42" s="5"/>
-      <c r="BI42" s="5"/>
-      <c r="BJ42" s="5"/>
-      <c r="BK42" s="5"/>
-      <c r="BL42" s="5"/>
-      <c r="BM42" s="5"/>
-      <c r="BN42" s="5"/>
-      <c r="BO42" s="5"/>
-      <c r="BP42" s="5"/>
-      <c r="BQ42" s="5"/>
-      <c r="BR42" s="5"/>
-      <c r="BS42" s="5"/>
-      <c r="BT42" s="5"/>
-      <c r="BU42" s="5"/>
-      <c r="BV42" s="5"/>
-      <c r="BW42" s="5"/>
-      <c r="BX42" s="5"/>
-      <c r="BY42" s="5"/>
-      <c r="BZ42" s="5"/>
-      <c r="CA42" s="5"/>
-      <c r="CB42" s="5"/>
-      <c r="CC42" s="5"/>
-      <c r="CD42" s="5"/>
-      <c r="CE42" s="5"/>
-      <c r="CF42" s="5"/>
-      <c r="CG42" s="5"/>
-      <c r="CH42" s="5"/>
-      <c r="CI42" s="5"/>
-      <c r="CJ42" s="5"/>
-      <c r="CK42" s="5"/>
-      <c r="CL42" s="5"/>
-      <c r="CM42" s="5"/>
-      <c r="CN42" s="5"/>
-      <c r="CO42" s="5"/>
-      <c r="CP42" s="5"/>
-      <c r="CQ42" s="5"/>
-      <c r="CR42" s="5"/>
-      <c r="CS42" s="5"/>
-      <c r="CT42" s="5"/>
-      <c r="CU42" s="5"/>
-      <c r="CV42" s="5"/>
-      <c r="CW42" s="5"/>
-      <c r="CX42" s="5"/>
-      <c r="CY42" s="5"/>
-      <c r="CZ42" s="5"/>
-      <c r="DA42" s="5"/>
-      <c r="DB42" s="5"/>
-      <c r="DC42" s="5"/>
-      <c r="DD42" s="5"/>
-      <c r="DE42" s="5"/>
-      <c r="DF42" s="5"/>
-      <c r="DG42" s="5"/>
-      <c r="DH42" s="5"/>
-      <c r="DI42" s="5"/>
-      <c r="DJ42" s="5"/>
-      <c r="DK42" s="5"/>
-      <c r="DL42" s="5"/>
-      <c r="DM42" s="5"/>
-      <c r="DN42" s="5"/>
-      <c r="DO42" s="5"/>
-      <c r="DP42" s="5"/>
-      <c r="DQ42" s="5"/>
-      <c r="DR42" s="5"/>
-      <c r="DS42" s="5"/>
-      <c r="DT42" s="5"/>
-      <c r="DU42" s="5"/>
-      <c r="DV42" s="5"/>
-      <c r="DW42" s="5"/>
-      <c r="DX42" s="5"/>
-      <c r="DY42" s="5"/>
-      <c r="DZ42" s="5"/>
-      <c r="EA42" s="5"/>
-      <c r="EB42" s="5"/>
-      <c r="EC42" s="5"/>
-      <c r="ED42" s="5"/>
-      <c r="EE42" s="5"/>
-      <c r="EF42" s="5"/>
-      <c r="EG42" s="5"/>
-      <c r="EH42" s="5"/>
-      <c r="EI42" s="5"/>
-      <c r="EJ42" s="5"/>
-      <c r="EK42" s="5"/>
-      <c r="EL42" s="5"/>
-      <c r="EM42" s="5"/>
-      <c r="EN42" s="5"/>
-      <c r="EO42" s="5"/>
-      <c r="EP42" s="5"/>
-      <c r="EQ42" s="5"/>
-      <c r="ER42" s="5"/>
-      <c r="ES42" s="5"/>
-      <c r="ET42" s="5"/>
-      <c r="EU42" s="5"/>
-      <c r="EV42" s="5"/>
-      <c r="EW42" s="5"/>
-      <c r="EX42" s="5"/>
-      <c r="EY42" s="5"/>
-      <c r="EZ42" s="5"/>
-      <c r="FA42" s="5"/>
-      <c r="FB42" s="5"/>
-      <c r="FC42" s="5"/>
-      <c r="FD42" s="5"/>
-      <c r="FE42" s="5"/>
-      <c r="FF42" s="5"/>
-      <c r="FG42" s="5"/>
-      <c r="FH42" s="5"/>
-      <c r="FI42" s="5"/>
-      <c r="FJ42" s="5"/>
-      <c r="FK42" s="5"/>
-      <c r="FL42" s="5"/>
-      <c r="FM42" s="5"/>
-      <c r="FN42" s="5"/>
+      <c r="B41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="14">
+        <v>2</v>
+      </c>
+      <c r="D41" s="14">
+        <v>3</v>
+      </c>
+      <c r="E41" s="13">
+        <f t="shared" ref="E41:E50" si="2">C41-D41</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="9"/>
+      <c r="B42" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="14">
+        <v>45</v>
+      </c>
+      <c r="D42" s="14">
+        <v>60</v>
+      </c>
+      <c r="E42" s="13">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
     </row>
     <row r="43" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="15"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="14">
+        <v>30</v>
+      </c>
+      <c r="D43" s="14">
+        <v>40</v>
+      </c>
+      <c r="E43" s="13">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
     </row>
     <row r="44" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="5"/>
-      <c r="X45" s="5"/>
-      <c r="Y45" s="5"/>
-      <c r="Z45" s="5"/>
-      <c r="AA45" s="5"/>
-      <c r="AB45" s="5"/>
-      <c r="AC45" s="5"/>
-      <c r="AD45" s="5"/>
-      <c r="AE45" s="5"/>
-      <c r="AF45" s="5"/>
-      <c r="AG45" s="5"/>
-      <c r="AH45" s="5"/>
-      <c r="AI45" s="5"/>
-      <c r="AJ45" s="5"/>
-      <c r="AK45" s="5"/>
-      <c r="AL45" s="5"/>
-      <c r="AM45" s="5"/>
-      <c r="AN45" s="5"/>
-      <c r="AO45" s="5"/>
-      <c r="AP45" s="5"/>
-      <c r="AQ45" s="5"/>
-      <c r="AR45" s="5"/>
-      <c r="AS45" s="5"/>
-      <c r="AT45" s="5"/>
-      <c r="AU45" s="5"/>
-      <c r="AV45" s="5"/>
-      <c r="AW45" s="5"/>
-      <c r="AX45" s="5"/>
-      <c r="AY45" s="5"/>
-      <c r="AZ45" s="5"/>
-      <c r="BA45" s="5"/>
-      <c r="BB45" s="5"/>
-      <c r="BC45" s="5"/>
-      <c r="BD45" s="5"/>
-      <c r="BE45" s="5"/>
-      <c r="BF45" s="5"/>
-      <c r="BG45" s="5"/>
-      <c r="BH45" s="5"/>
-      <c r="BI45" s="5"/>
-      <c r="BJ45" s="5"/>
-      <c r="BK45" s="5"/>
-      <c r="BL45" s="5"/>
-      <c r="BM45" s="5"/>
-      <c r="BN45" s="5"/>
-      <c r="BO45" s="5"/>
-      <c r="BP45" s="5"/>
-      <c r="BQ45" s="5"/>
-      <c r="BR45" s="5"/>
-      <c r="BS45" s="5"/>
-      <c r="BT45" s="5"/>
-      <c r="BU45" s="5"/>
-      <c r="BV45" s="5"/>
-      <c r="BW45" s="5"/>
-      <c r="BX45" s="5"/>
-      <c r="BY45" s="5"/>
-      <c r="BZ45" s="5"/>
-      <c r="CA45" s="5"/>
-      <c r="CB45" s="5"/>
-      <c r="CC45" s="5"/>
-      <c r="CD45" s="5"/>
-      <c r="CE45" s="5"/>
-      <c r="CF45" s="5"/>
-      <c r="CG45" s="5"/>
-      <c r="CH45" s="5"/>
-      <c r="CI45" s="5"/>
-      <c r="CJ45" s="5"/>
-      <c r="CK45" s="5"/>
-      <c r="CL45" s="5"/>
-      <c r="CM45" s="5"/>
-      <c r="CN45" s="5"/>
-      <c r="CO45" s="5"/>
-      <c r="CP45" s="5"/>
-      <c r="CQ45" s="5"/>
-      <c r="CR45" s="5"/>
-      <c r="CS45" s="5"/>
-      <c r="CT45" s="5"/>
-      <c r="CU45" s="5"/>
-      <c r="CV45" s="5"/>
-      <c r="CW45" s="5"/>
-      <c r="CX45" s="5"/>
-      <c r="CY45" s="5"/>
-      <c r="CZ45" s="5"/>
-      <c r="DA45" s="5"/>
-      <c r="DB45" s="5"/>
-      <c r="DC45" s="5"/>
-      <c r="DD45" s="5"/>
-      <c r="DE45" s="5"/>
-      <c r="DF45" s="5"/>
-      <c r="DG45" s="5"/>
-      <c r="DH45" s="5"/>
-      <c r="DI45" s="5"/>
-      <c r="DJ45" s="5"/>
-      <c r="DK45" s="5"/>
-      <c r="DL45" s="5"/>
-      <c r="DM45" s="5"/>
-      <c r="DN45" s="5"/>
-      <c r="DO45" s="5"/>
-      <c r="DP45" s="5"/>
-      <c r="DQ45" s="5"/>
-      <c r="DR45" s="5"/>
-      <c r="DS45" s="5"/>
-      <c r="DT45" s="5"/>
-      <c r="DU45" s="5"/>
-      <c r="DV45" s="5"/>
-      <c r="DW45" s="5"/>
-      <c r="DX45" s="5"/>
-      <c r="DY45" s="5"/>
-      <c r="DZ45" s="5"/>
-      <c r="EA45" s="5"/>
-      <c r="EB45" s="5"/>
-      <c r="EC45" s="5"/>
-      <c r="ED45" s="5"/>
-      <c r="EE45" s="5"/>
-      <c r="EF45" s="5"/>
-      <c r="EG45" s="5"/>
-      <c r="EH45" s="5"/>
-      <c r="EI45" s="5"/>
-      <c r="EJ45" s="5"/>
-      <c r="EK45" s="5"/>
-      <c r="EL45" s="5"/>
-      <c r="EM45" s="5"/>
-      <c r="EN45" s="5"/>
-      <c r="EO45" s="5"/>
-      <c r="EP45" s="5"/>
-      <c r="EQ45" s="5"/>
-      <c r="ER45" s="5"/>
-      <c r="ES45" s="5"/>
-      <c r="ET45" s="5"/>
-      <c r="EU45" s="5"/>
-      <c r="EV45" s="5"/>
-      <c r="EW45" s="5"/>
-      <c r="EX45" s="5"/>
-      <c r="EY45" s="5"/>
-      <c r="EZ45" s="5"/>
-      <c r="FA45" s="5"/>
-      <c r="FB45" s="5"/>
-      <c r="FC45" s="5"/>
-      <c r="FD45" s="5"/>
-      <c r="FE45" s="5"/>
-      <c r="FF45" s="5"/>
-      <c r="FG45" s="5"/>
-      <c r="FH45" s="5"/>
-      <c r="FI45" s="5"/>
-      <c r="FJ45" s="5"/>
-      <c r="FK45" s="5"/>
-      <c r="FL45" s="5"/>
-      <c r="FM45" s="5"/>
-      <c r="FN45" s="5"/>
+      <c r="B44" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="14">
+        <v>60</v>
+      </c>
+      <c r="D44" s="14">
+        <v>70</v>
+      </c>
+      <c r="E44" s="13">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="9"/>
+      <c r="B45" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="14">
+        <v>10</v>
+      </c>
+      <c r="D45" s="14">
+        <v>5</v>
+      </c>
+      <c r="E45" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="14">
+        <v>30</v>
+      </c>
+      <c r="D46" s="14">
+        <v>45</v>
+      </c>
+      <c r="E46" s="13">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+      <c r="B47" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="14">
+        <v>15</v>
+      </c>
+      <c r="D47" s="14">
+        <v>15</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="9"/>
+      <c r="B48" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="14">
+        <v>10</v>
+      </c>
+      <c r="D48" s="14">
+        <v>10</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9"/>
+      <c r="B49" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="14">
+        <v>65</v>
+      </c>
+      <c r="D49" s="14">
+        <v>70</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="9"/>
+      <c r="B50" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="14">
+        <v>30</v>
+      </c>
+      <c r="D50" s="14">
+        <v>30</v>
+      </c>
+      <c r="E50" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="5"/>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="5"/>
+      <c r="AF51" s="5"/>
+      <c r="AG51" s="5"/>
+      <c r="AH51" s="5"/>
+      <c r="AI51" s="5"/>
+      <c r="AJ51" s="5"/>
+      <c r="AK51" s="5"/>
+      <c r="AL51" s="5"/>
+      <c r="AM51" s="5"/>
+      <c r="AN51" s="5"/>
+      <c r="AO51" s="5"/>
+      <c r="AP51" s="5"/>
+      <c r="AQ51" s="5"/>
+      <c r="AR51" s="5"/>
+      <c r="AS51" s="5"/>
+      <c r="AT51" s="5"/>
+      <c r="AU51" s="5"/>
+      <c r="AV51" s="5"/>
+      <c r="AW51" s="5"/>
+      <c r="AX51" s="5"/>
+      <c r="AY51" s="5"/>
+      <c r="AZ51" s="5"/>
+      <c r="BA51" s="5"/>
+      <c r="BB51" s="5"/>
+      <c r="BC51" s="5"/>
+      <c r="BD51" s="5"/>
+      <c r="BE51" s="5"/>
+      <c r="BF51" s="5"/>
+      <c r="BG51" s="5"/>
+      <c r="BH51" s="5"/>
+      <c r="BI51" s="5"/>
+      <c r="BJ51" s="5"/>
+      <c r="BK51" s="5"/>
+      <c r="BL51" s="5"/>
+      <c r="BM51" s="5"/>
+      <c r="BN51" s="5"/>
+      <c r="BO51" s="5"/>
+      <c r="BP51" s="5"/>
+      <c r="BQ51" s="5"/>
+      <c r="BR51" s="5"/>
+      <c r="BS51" s="5"/>
+      <c r="BT51" s="5"/>
+      <c r="BU51" s="5"/>
+      <c r="BV51" s="5"/>
+      <c r="BW51" s="5"/>
+      <c r="BX51" s="5"/>
+      <c r="BY51" s="5"/>
+      <c r="BZ51" s="5"/>
+      <c r="CA51" s="5"/>
+      <c r="CB51" s="5"/>
+      <c r="CC51" s="5"/>
+      <c r="CD51" s="5"/>
+      <c r="CE51" s="5"/>
+      <c r="CF51" s="5"/>
+      <c r="CG51" s="5"/>
+      <c r="CH51" s="5"/>
+      <c r="CI51" s="5"/>
+      <c r="CJ51" s="5"/>
+      <c r="CK51" s="5"/>
+      <c r="CL51" s="5"/>
+      <c r="CM51" s="5"/>
+      <c r="CN51" s="5"/>
+      <c r="CO51" s="5"/>
+      <c r="CP51" s="5"/>
+      <c r="CQ51" s="5"/>
+      <c r="CR51" s="5"/>
+      <c r="CS51" s="5"/>
+      <c r="CT51" s="5"/>
+      <c r="CU51" s="5"/>
+      <c r="CV51" s="5"/>
+      <c r="CW51" s="5"/>
+      <c r="CX51" s="5"/>
+      <c r="CY51" s="5"/>
+      <c r="CZ51" s="5"/>
+      <c r="DA51" s="5"/>
+      <c r="DB51" s="5"/>
+      <c r="DC51" s="5"/>
+      <c r="DD51" s="5"/>
+      <c r="DE51" s="5"/>
+      <c r="DF51" s="5"/>
+      <c r="DG51" s="5"/>
+      <c r="DH51" s="5"/>
+      <c r="DI51" s="5"/>
+      <c r="DJ51" s="5"/>
+      <c r="DK51" s="5"/>
+      <c r="DL51" s="5"/>
+      <c r="DM51" s="5"/>
+      <c r="DN51" s="5"/>
+      <c r="DO51" s="5"/>
+      <c r="DP51" s="5"/>
+      <c r="DQ51" s="5"/>
+      <c r="DR51" s="5"/>
+      <c r="DS51" s="5"/>
+      <c r="DT51" s="5"/>
+      <c r="DU51" s="5"/>
+      <c r="DV51" s="5"/>
+      <c r="DW51" s="5"/>
+      <c r="DX51" s="5"/>
+      <c r="DY51" s="5"/>
+      <c r="DZ51" s="5"/>
+      <c r="EA51" s="5"/>
+      <c r="EB51" s="5"/>
+      <c r="EC51" s="5"/>
+      <c r="ED51" s="5"/>
+      <c r="EE51" s="5"/>
+      <c r="EF51" s="5"/>
+      <c r="EG51" s="5"/>
+      <c r="EH51" s="5"/>
+      <c r="EI51" s="5"/>
+      <c r="EJ51" s="5"/>
+      <c r="EK51" s="5"/>
+      <c r="EL51" s="5"/>
+      <c r="EM51" s="5"/>
+      <c r="EN51" s="5"/>
+      <c r="EO51" s="5"/>
+      <c r="EP51" s="5"/>
+      <c r="EQ51" s="5"/>
+      <c r="ER51" s="5"/>
+      <c r="ES51" s="5"/>
+      <c r="ET51" s="5"/>
+      <c r="EU51" s="5"/>
+      <c r="EV51" s="5"/>
+      <c r="EW51" s="5"/>
+      <c r="EX51" s="5"/>
+      <c r="EY51" s="5"/>
+      <c r="EZ51" s="5"/>
+      <c r="FA51" s="5"/>
+      <c r="FB51" s="5"/>
+      <c r="FC51" s="5"/>
+      <c r="FD51" s="5"/>
+      <c r="FE51" s="5"/>
+      <c r="FF51" s="5"/>
+      <c r="FG51" s="5"/>
+      <c r="FH51" s="5"/>
+      <c r="FI51" s="5"/>
+      <c r="FJ51" s="5"/>
+      <c r="FK51" s="5"/>
+      <c r="FL51" s="5"/>
+      <c r="FM51" s="5"/>
+      <c r="FN51" s="5"/>
+    </row>
+    <row r="52" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:170" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="9"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="1:170" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="5"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="5"/>
+      <c r="AE54" s="5"/>
+      <c r="AF54" s="5"/>
+      <c r="AG54" s="5"/>
+      <c r="AH54" s="5"/>
+      <c r="AI54" s="5"/>
+      <c r="AJ54" s="5"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="5"/>
+      <c r="AM54" s="5"/>
+      <c r="AN54" s="5"/>
+      <c r="AO54" s="5"/>
+      <c r="AP54" s="5"/>
+      <c r="AQ54" s="5"/>
+      <c r="AR54" s="5"/>
+      <c r="AS54" s="5"/>
+      <c r="AT54" s="5"/>
+      <c r="AU54" s="5"/>
+      <c r="AV54" s="5"/>
+      <c r="AW54" s="5"/>
+      <c r="AX54" s="5"/>
+      <c r="AY54" s="5"/>
+      <c r="AZ54" s="5"/>
+      <c r="BA54" s="5"/>
+      <c r="BB54" s="5"/>
+      <c r="BC54" s="5"/>
+      <c r="BD54" s="5"/>
+      <c r="BE54" s="5"/>
+      <c r="BF54" s="5"/>
+      <c r="BG54" s="5"/>
+      <c r="BH54" s="5"/>
+      <c r="BI54" s="5"/>
+      <c r="BJ54" s="5"/>
+      <c r="BK54" s="5"/>
+      <c r="BL54" s="5"/>
+      <c r="BM54" s="5"/>
+      <c r="BN54" s="5"/>
+      <c r="BO54" s="5"/>
+      <c r="BP54" s="5"/>
+      <c r="BQ54" s="5"/>
+      <c r="BR54" s="5"/>
+      <c r="BS54" s="5"/>
+      <c r="BT54" s="5"/>
+      <c r="BU54" s="5"/>
+      <c r="BV54" s="5"/>
+      <c r="BW54" s="5"/>
+      <c r="BX54" s="5"/>
+      <c r="BY54" s="5"/>
+      <c r="BZ54" s="5"/>
+      <c r="CA54" s="5"/>
+      <c r="CB54" s="5"/>
+      <c r="CC54" s="5"/>
+      <c r="CD54" s="5"/>
+      <c r="CE54" s="5"/>
+      <c r="CF54" s="5"/>
+      <c r="CG54" s="5"/>
+      <c r="CH54" s="5"/>
+      <c r="CI54" s="5"/>
+      <c r="CJ54" s="5"/>
+      <c r="CK54" s="5"/>
+      <c r="CL54" s="5"/>
+      <c r="CM54" s="5"/>
+      <c r="CN54" s="5"/>
+      <c r="CO54" s="5"/>
+      <c r="CP54" s="5"/>
+      <c r="CQ54" s="5"/>
+      <c r="CR54" s="5"/>
+      <c r="CS54" s="5"/>
+      <c r="CT54" s="5"/>
+      <c r="CU54" s="5"/>
+      <c r="CV54" s="5"/>
+      <c r="CW54" s="5"/>
+      <c r="CX54" s="5"/>
+      <c r="CY54" s="5"/>
+      <c r="CZ54" s="5"/>
+      <c r="DA54" s="5"/>
+      <c r="DB54" s="5"/>
+      <c r="DC54" s="5"/>
+      <c r="DD54" s="5"/>
+      <c r="DE54" s="5"/>
+      <c r="DF54" s="5"/>
+      <c r="DG54" s="5"/>
+      <c r="DH54" s="5"/>
+      <c r="DI54" s="5"/>
+      <c r="DJ54" s="5"/>
+      <c r="DK54" s="5"/>
+      <c r="DL54" s="5"/>
+      <c r="DM54" s="5"/>
+      <c r="DN54" s="5"/>
+      <c r="DO54" s="5"/>
+      <c r="DP54" s="5"/>
+      <c r="DQ54" s="5"/>
+      <c r="DR54" s="5"/>
+      <c r="DS54" s="5"/>
+      <c r="DT54" s="5"/>
+      <c r="DU54" s="5"/>
+      <c r="DV54" s="5"/>
+      <c r="DW54" s="5"/>
+      <c r="DX54" s="5"/>
+      <c r="DY54" s="5"/>
+      <c r="DZ54" s="5"/>
+      <c r="EA54" s="5"/>
+      <c r="EB54" s="5"/>
+      <c r="EC54" s="5"/>
+      <c r="ED54" s="5"/>
+      <c r="EE54" s="5"/>
+      <c r="EF54" s="5"/>
+      <c r="EG54" s="5"/>
+      <c r="EH54" s="5"/>
+      <c r="EI54" s="5"/>
+      <c r="EJ54" s="5"/>
+      <c r="EK54" s="5"/>
+      <c r="EL54" s="5"/>
+      <c r="EM54" s="5"/>
+      <c r="EN54" s="5"/>
+      <c r="EO54" s="5"/>
+      <c r="EP54" s="5"/>
+      <c r="EQ54" s="5"/>
+      <c r="ER54" s="5"/>
+      <c r="ES54" s="5"/>
+      <c r="ET54" s="5"/>
+      <c r="EU54" s="5"/>
+      <c r="EV54" s="5"/>
+      <c r="EW54" s="5"/>
+      <c r="EX54" s="5"/>
+      <c r="EY54" s="5"/>
+      <c r="EZ54" s="5"/>
+      <c r="FA54" s="5"/>
+      <c r="FB54" s="5"/>
+      <c r="FC54" s="5"/>
+      <c r="FD54" s="5"/>
+      <c r="FE54" s="5"/>
+      <c r="FF54" s="5"/>
+      <c r="FG54" s="5"/>
+      <c r="FH54" s="5"/>
+      <c r="FI54" s="5"/>
+      <c r="FJ54" s="5"/>
+      <c r="FK54" s="5"/>
+      <c r="FL54" s="5"/>
+      <c r="FM54" s="5"/>
+      <c r="FN54" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A54:E54"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>

</xml_diff>